<commit_message>
Update LSA Data Dictionary FY2024.xlsx
Closes #1228
</commit_message>
<xml_diff>
--- a/LSA Data Dictionary FY2024.xlsx
+++ b/LSA Data Dictionary FY2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://squarepegdata-my.sharepoint.com/personal/molly_squarepegdata_com/Documents/GitHub/LSASampleCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{4C794D6F-E862-4F2C-98E1-131F5B0D33CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F7648DF-F483-40E6-B16B-0660982D1918}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{4C794D6F-E862-4F2C-98E1-131F5B0D33CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{329C507A-3AFF-4D8D-B7E7-E4B7A338D72A}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-7455" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B02B7233-7B9E-4318-BE1B-2F97AB3B1B83}"/>
   </bookViews>
@@ -4808,7 +4808,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -4883,6 +4883,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
@@ -4906,6 +4913,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13278,7 +13289,8 @@
   <cols>
     <col min="2" max="2" width="19.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="95.53125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="28" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -19987,7 +19999,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="480" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="480" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A480">
         <v>28</v>
       </c>
@@ -20001,7 +20013,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="481" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="481" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A481">
         <v>28</v>
       </c>
@@ -21456,7 +21468,7 @@
       <c r="D584" t="s">
         <v>413</v>
       </c>
-      <c r="N584" s="22"/>
+      <c r="N584" s="29"/>
     </row>
     <row r="585" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A585">
@@ -21471,7 +21483,7 @@
       <c r="D585" t="s">
         <v>367</v>
       </c>
-      <c r="N585" s="22"/>
+      <c r="N585" s="29"/>
     </row>
     <row r="586" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A586">
@@ -21486,7 +21498,7 @@
       <c r="D586" t="s">
         <v>368</v>
       </c>
-      <c r="N586" s="22"/>
+      <c r="N586" s="29"/>
     </row>
     <row r="587" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A587">
@@ -21501,7 +21513,7 @@
       <c r="D587" t="s">
         <v>369</v>
       </c>
-      <c r="N587" s="22"/>
+      <c r="N587" s="29"/>
     </row>
     <row r="588" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A588">
@@ -21516,7 +21528,7 @@
       <c r="D588" t="s">
         <v>370</v>
       </c>
-      <c r="N588" s="22"/>
+      <c r="N588" s="29"/>
     </row>
     <row r="589" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A589">
@@ -21531,7 +21543,7 @@
       <c r="D589" t="s">
         <v>371</v>
       </c>
-      <c r="N589" s="22"/>
+      <c r="N589" s="29"/>
     </row>
     <row r="590" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A590">
@@ -21546,7 +21558,7 @@
       <c r="D590" t="s">
         <v>372</v>
       </c>
-      <c r="N590" s="22"/>
+      <c r="N590" s="29"/>
     </row>
     <row r="591" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A591">
@@ -21561,7 +21573,7 @@
       <c r="D591" t="s">
         <v>373</v>
       </c>
-      <c r="N591" s="22"/>
+      <c r="N591" s="29"/>
     </row>
     <row r="592" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A592">
@@ -21576,7 +21588,7 @@
       <c r="D592" t="s">
         <v>374</v>
       </c>
-      <c r="N592" s="22"/>
+      <c r="N592" s="29"/>
     </row>
     <row r="593" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A593">
@@ -21591,7 +21603,7 @@
       <c r="D593" t="s">
         <v>375</v>
       </c>
-      <c r="N593" s="22"/>
+      <c r="N593" s="29"/>
     </row>
     <row r="594" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A594">
@@ -22138,7 +22150,7 @@
       <c r="D632" t="s">
         <v>1151</v>
       </c>
-      <c r="F632" s="22"/>
+      <c r="F632" s="29"/>
     </row>
     <row r="633" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A633">
@@ -22153,7 +22165,7 @@
       <c r="D633" t="s">
         <v>1152</v>
       </c>
-      <c r="F633" s="22"/>
+      <c r="F633" s="29"/>
     </row>
     <row r="634" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A634">
@@ -22168,7 +22180,7 @@
       <c r="D634" t="s">
         <v>1153</v>
       </c>
-      <c r="F634" s="22"/>
+      <c r="F634" s="29"/>
     </row>
     <row r="635" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A635">
@@ -22183,7 +22195,7 @@
       <c r="D635" t="s">
         <v>1154</v>
       </c>
-      <c r="F635" s="22"/>
+      <c r="F635" s="29"/>
     </row>
     <row r="636" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A636">
@@ -22198,7 +22210,7 @@
       <c r="D636" t="s">
         <v>1155</v>
       </c>
-      <c r="F636" s="22"/>
+      <c r="F636" s="29"/>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A637">
@@ -22213,7 +22225,7 @@
       <c r="D637" t="s">
         <v>1156</v>
       </c>
-      <c r="F637" s="22"/>
+      <c r="F637" s="29"/>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A638">
@@ -22228,7 +22240,7 @@
       <c r="D638" t="s">
         <v>1157</v>
       </c>
-      <c r="F638" s="22"/>
+      <c r="F638" s="29"/>
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A639">
@@ -22243,7 +22255,7 @@
       <c r="D639" t="s">
         <v>1158</v>
       </c>
-      <c r="F639" s="22"/>
+      <c r="F639" s="29"/>
     </row>
     <row r="640" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A640">
@@ -22258,7 +22270,7 @@
       <c r="D640" t="s">
         <v>1159</v>
       </c>
-      <c r="F640" s="22"/>
+      <c r="F640" s="29"/>
     </row>
     <row r="641" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A641">
@@ -22273,7 +22285,7 @@
       <c r="D641" t="s">
         <v>1160</v>
       </c>
-      <c r="F641" s="22"/>
+      <c r="F641" s="29"/>
     </row>
     <row r="642" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A642">
@@ -22288,7 +22300,7 @@
       <c r="D642" t="s">
         <v>1161</v>
       </c>
-      <c r="F642" s="22"/>
+      <c r="F642" s="29"/>
     </row>
     <row r="643" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A643">
@@ -22303,7 +22315,7 @@
       <c r="D643" t="s">
         <v>1162</v>
       </c>
-      <c r="F643" s="22"/>
+      <c r="F643" s="29"/>
     </row>
     <row r="644" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A644">
@@ -22318,7 +22330,7 @@
       <c r="D644" t="s">
         <v>1163</v>
       </c>
-      <c r="F644" s="22"/>
+      <c r="F644" s="29"/>
     </row>
     <row r="645" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A645">
@@ -22333,7 +22345,7 @@
       <c r="D645" t="s">
         <v>1164</v>
       </c>
-      <c r="F645" s="22"/>
+      <c r="F645" s="29"/>
     </row>
     <row r="646" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A646">
@@ -22348,7 +22360,7 @@
       <c r="D646" t="s">
         <v>1165</v>
       </c>
-      <c r="F646" s="22"/>
+      <c r="F646" s="29"/>
     </row>
     <row r="647" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A647">
@@ -22363,7 +22375,7 @@
       <c r="D647" t="s">
         <v>1166</v>
       </c>
-      <c r="F647" s="22"/>
+      <c r="F647" s="29"/>
     </row>
     <row r="648" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A648">
@@ -22378,7 +22390,7 @@
       <c r="D648" t="s">
         <v>1167</v>
       </c>
-      <c r="F648" s="22"/>
+      <c r="F648" s="29"/>
     </row>
     <row r="649" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A649">
@@ -22393,7 +22405,7 @@
       <c r="D649" t="s">
         <v>1168</v>
       </c>
-      <c r="F649" s="22"/>
+      <c r="F649" s="29"/>
     </row>
     <row r="650" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A650">
@@ -22408,7 +22420,7 @@
       <c r="D650" t="s">
         <v>1169</v>
       </c>
-      <c r="F650" s="22"/>
+      <c r="F650" s="29"/>
     </row>
     <row r="651" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A651">
@@ -22423,7 +22435,7 @@
       <c r="D651" t="s">
         <v>1170</v>
       </c>
-      <c r="F651" s="22"/>
+      <c r="F651" s="29"/>
     </row>
     <row r="652" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A652">
@@ -22438,7 +22450,7 @@
       <c r="D652" t="s">
         <v>1171</v>
       </c>
-      <c r="F652" s="22"/>
+      <c r="F652" s="29"/>
     </row>
     <row r="653" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A653">
@@ -22467,7 +22479,7 @@
       <c r="D654" t="s">
         <v>382</v>
       </c>
-      <c r="F654" s="22"/>
+      <c r="F654" s="29"/>
     </row>
     <row r="655" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A655">
@@ -22566,7 +22578,7 @@
       <c r="D661" t="s">
         <v>1175</v>
       </c>
-      <c r="F661" s="22"/>
+      <c r="F661" s="29"/>
     </row>
     <row r="662" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A662">
@@ -22581,7 +22593,7 @@
       <c r="D662" t="s">
         <v>1176</v>
       </c>
-      <c r="F662" s="22"/>
+      <c r="F662" s="29"/>
     </row>
     <row r="663" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A663">
@@ -22596,7 +22608,7 @@
       <c r="D663" t="s">
         <v>1177</v>
       </c>
-      <c r="F663" s="22"/>
+      <c r="F663" s="29"/>
     </row>
     <row r="664" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A664">
@@ -22611,7 +22623,7 @@
       <c r="D664" t="s">
         <v>1178</v>
       </c>
-      <c r="F664" s="22"/>
+      <c r="F664" s="29"/>
     </row>
     <row r="665" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A665">
@@ -22626,7 +22638,7 @@
       <c r="D665" t="s">
         <v>1179</v>
       </c>
-      <c r="F665" s="22"/>
+      <c r="F665" s="29"/>
     </row>
     <row r="666" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A666">
@@ -22641,7 +22653,7 @@
       <c r="D666" t="s">
         <v>1180</v>
       </c>
-      <c r="F666" s="22"/>
+      <c r="F666" s="29"/>
     </row>
     <row r="667" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A667">
@@ -22656,7 +22668,7 @@
       <c r="D667" t="s">
         <v>1181</v>
       </c>
-      <c r="F667" s="22"/>
+      <c r="F667" s="29"/>
     </row>
     <row r="668" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A668">
@@ -22671,7 +22683,7 @@
       <c r="D668" t="s">
         <v>1182</v>
       </c>
-      <c r="F668" s="22"/>
+      <c r="F668" s="29"/>
     </row>
     <row r="669" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A669">
@@ -22686,7 +22698,7 @@
       <c r="D669" t="s">
         <v>1183</v>
       </c>
-      <c r="F669" s="22"/>
+      <c r="F669" s="29"/>
     </row>
     <row r="670" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A670">
@@ -22701,7 +22713,7 @@
       <c r="D670" t="s">
         <v>1184</v>
       </c>
-      <c r="F670" s="22"/>
+      <c r="F670" s="29"/>
     </row>
     <row r="671" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A671">
@@ -22716,7 +22728,7 @@
       <c r="D671" t="s">
         <v>1185</v>
       </c>
-      <c r="F671" s="22"/>
+      <c r="F671" s="29"/>
     </row>
     <row r="672" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A672">
@@ -22731,7 +22743,7 @@
       <c r="D672" t="s">
         <v>1186</v>
       </c>
-      <c r="F672" s="22"/>
+      <c r="F672" s="29"/>
     </row>
     <row r="673" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A673">
@@ -22746,7 +22758,7 @@
       <c r="D673" t="s">
         <v>1187</v>
       </c>
-      <c r="F673" s="22"/>
+      <c r="F673" s="29"/>
     </row>
     <row r="674" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A674">
@@ -22761,7 +22773,7 @@
       <c r="D674" t="s">
         <v>1188</v>
       </c>
-      <c r="F674" s="22"/>
+      <c r="F674" s="29"/>
     </row>
     <row r="675" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A675">
@@ -22776,7 +22788,7 @@
       <c r="D675" t="s">
         <v>1189</v>
       </c>
-      <c r="F675" s="22"/>
+      <c r="F675" s="29"/>
     </row>
     <row r="676" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A676">
@@ -22791,7 +22803,7 @@
       <c r="D676" t="s">
         <v>1190</v>
       </c>
-      <c r="F676" s="22"/>
+      <c r="F676" s="29"/>
     </row>
     <row r="677" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A677">
@@ -22806,7 +22818,7 @@
       <c r="D677" t="s">
         <v>1191</v>
       </c>
-      <c r="F677" s="22"/>
+      <c r="F677" s="29"/>
     </row>
     <row r="678" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A678">
@@ -22821,7 +22833,7 @@
       <c r="D678" t="s">
         <v>1192</v>
       </c>
-      <c r="F678" s="22"/>
+      <c r="F678" s="29"/>
     </row>
     <row r="679" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A679">
@@ -22836,7 +22848,7 @@
       <c r="D679" t="s">
         <v>1193</v>
       </c>
-      <c r="F679" s="22"/>
+      <c r="F679" s="29"/>
     </row>
     <row r="680" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A680">
@@ -22851,7 +22863,7 @@
       <c r="D680" t="s">
         <v>1194</v>
       </c>
-      <c r="F680" s="22"/>
+      <c r="F680" s="29"/>
     </row>
     <row r="681" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A681">
@@ -22866,7 +22878,7 @@
       <c r="D681" t="s">
         <v>1195</v>
       </c>
-      <c r="F681" s="22"/>
+      <c r="F681" s="29"/>
     </row>
     <row r="682" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A682">
@@ -22881,7 +22893,7 @@
       <c r="D682" t="s">
         <v>1196</v>
       </c>
-      <c r="F682" s="22"/>
+      <c r="F682" s="29"/>
     </row>
     <row r="683" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A683">
@@ -23022,7 +23034,7 @@
       <c r="D692" t="s">
         <v>1201</v>
       </c>
-      <c r="F692" s="22"/>
+      <c r="F692" s="29"/>
     </row>
     <row r="693" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A693">
@@ -23037,7 +23049,7 @@
       <c r="D693" t="s">
         <v>1202</v>
       </c>
-      <c r="F693" s="22"/>
+      <c r="F693" s="29"/>
     </row>
     <row r="694" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A694">
@@ -23052,7 +23064,7 @@
       <c r="D694" t="s">
         <v>1203</v>
       </c>
-      <c r="F694" s="22"/>
+      <c r="F694" s="29"/>
     </row>
     <row r="695" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A695">
@@ -23067,7 +23079,7 @@
       <c r="D695" t="s">
         <v>1204</v>
       </c>
-      <c r="F695" s="22"/>
+      <c r="F695" s="29"/>
     </row>
     <row r="696" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A696">
@@ -23082,7 +23094,7 @@
       <c r="D696" t="s">
         <v>1205</v>
       </c>
-      <c r="F696" s="22"/>
+      <c r="F696" s="29"/>
     </row>
     <row r="697" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A697">
@@ -23097,7 +23109,7 @@
       <c r="D697" t="s">
         <v>1206</v>
       </c>
-      <c r="F697" s="22"/>
+      <c r="F697" s="29"/>
     </row>
     <row r="698" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A698">
@@ -23112,7 +23124,7 @@
       <c r="D698" t="s">
         <v>1207</v>
       </c>
-      <c r="F698" s="22"/>
+      <c r="F698" s="29"/>
     </row>
     <row r="699" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A699">
@@ -23127,7 +23139,7 @@
       <c r="D699" t="s">
         <v>1208</v>
       </c>
-      <c r="F699" s="22"/>
+      <c r="F699" s="29"/>
     </row>
     <row r="700" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A700">
@@ -23142,7 +23154,7 @@
       <c r="D700" t="s">
         <v>1209</v>
       </c>
-      <c r="F700" s="22"/>
+      <c r="F700" s="29"/>
     </row>
     <row r="701" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A701">
@@ -23157,7 +23169,7 @@
       <c r="D701" t="s">
         <v>1210</v>
       </c>
-      <c r="F701" s="22"/>
+      <c r="F701" s="29"/>
     </row>
     <row r="702" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A702">
@@ -23172,7 +23184,7 @@
       <c r="D702" t="s">
         <v>1211</v>
       </c>
-      <c r="F702" s="22"/>
+      <c r="F702" s="29"/>
     </row>
     <row r="703" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A703">
@@ -23187,7 +23199,7 @@
       <c r="D703" t="s">
         <v>1212</v>
       </c>
-      <c r="F703" s="22"/>
+      <c r="F703" s="29"/>
     </row>
     <row r="704" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A704">
@@ -23202,7 +23214,7 @@
       <c r="D704" t="s">
         <v>1213</v>
       </c>
-      <c r="F704" s="22"/>
+      <c r="F704" s="29"/>
     </row>
     <row r="705" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A705">
@@ -23217,7 +23229,7 @@
       <c r="D705" t="s">
         <v>1214</v>
       </c>
-      <c r="F705" s="22"/>
+      <c r="F705" s="29"/>
     </row>
     <row r="706" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A706">
@@ -23232,7 +23244,7 @@
       <c r="D706" t="s">
         <v>1215</v>
       </c>
-      <c r="F706" s="22"/>
+      <c r="F706" s="29"/>
     </row>
     <row r="707" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A707">
@@ -23247,7 +23259,7 @@
       <c r="D707" t="s">
         <v>1216</v>
       </c>
-      <c r="F707" s="22"/>
+      <c r="F707" s="29"/>
     </row>
     <row r="708" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A708">
@@ -23262,7 +23274,7 @@
       <c r="D708" t="s">
         <v>1217</v>
       </c>
-      <c r="F708" s="22"/>
+      <c r="F708" s="29"/>
     </row>
     <row r="709" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A709">
@@ -23277,7 +23289,7 @@
       <c r="D709" t="s">
         <v>1218</v>
       </c>
-      <c r="F709" s="22"/>
+      <c r="F709" s="29"/>
     </row>
     <row r="710" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A710">
@@ -23292,7 +23304,7 @@
       <c r="D710" t="s">
         <v>1219</v>
       </c>
-      <c r="F710" s="22"/>
+      <c r="F710" s="29"/>
     </row>
     <row r="711" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A711">
@@ -23307,7 +23319,7 @@
       <c r="D711" t="s">
         <v>1220</v>
       </c>
-      <c r="F711" s="22"/>
+      <c r="F711" s="29"/>
     </row>
     <row r="712" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A712">
@@ -23322,7 +23334,7 @@
       <c r="D712" t="s">
         <v>1221</v>
       </c>
-      <c r="F712" s="22"/>
+      <c r="F712" s="29"/>
     </row>
     <row r="713" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A713">
@@ -23337,7 +23349,7 @@
       <c r="D713" t="s">
         <v>1222</v>
       </c>
-      <c r="F713" s="22"/>
+      <c r="F713" s="29"/>
     </row>
     <row r="714" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A714">
@@ -23478,7 +23490,7 @@
       <c r="D723" t="s">
         <v>1227</v>
       </c>
-      <c r="F723" s="22"/>
+      <c r="F723" s="29"/>
     </row>
     <row r="724" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A724">
@@ -23493,7 +23505,7 @@
       <c r="D724" t="s">
         <v>1228</v>
       </c>
-      <c r="F724" s="22"/>
+      <c r="F724" s="29"/>
     </row>
     <row r="725" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A725">
@@ -23508,7 +23520,7 @@
       <c r="D725" t="s">
         <v>1229</v>
       </c>
-      <c r="F725" s="22"/>
+      <c r="F725" s="29"/>
     </row>
     <row r="726" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A726">
@@ -23523,7 +23535,7 @@
       <c r="D726" t="s">
         <v>1230</v>
       </c>
-      <c r="F726" s="22"/>
+      <c r="F726" s="29"/>
     </row>
     <row r="727" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A727">
@@ -23538,7 +23550,7 @@
       <c r="D727" t="s">
         <v>1231</v>
       </c>
-      <c r="F727" s="22"/>
+      <c r="F727" s="29"/>
     </row>
     <row r="728" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A728">
@@ -23553,7 +23565,7 @@
       <c r="D728" t="s">
         <v>1232</v>
       </c>
-      <c r="F728" s="22"/>
+      <c r="F728" s="29"/>
     </row>
     <row r="729" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A729">
@@ -23568,7 +23580,7 @@
       <c r="D729" t="s">
         <v>1233</v>
       </c>
-      <c r="F729" s="22"/>
+      <c r="F729" s="29"/>
     </row>
     <row r="730" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A730">
@@ -23583,7 +23595,7 @@
       <c r="D730" t="s">
         <v>1234</v>
       </c>
-      <c r="F730" s="22"/>
+      <c r="F730" s="29"/>
     </row>
     <row r="731" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A731">
@@ -23598,7 +23610,7 @@
       <c r="D731" t="s">
         <v>1235</v>
       </c>
-      <c r="F731" s="22"/>
+      <c r="F731" s="29"/>
     </row>
     <row r="732" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A732">
@@ -23613,7 +23625,7 @@
       <c r="D732" t="s">
         <v>1236</v>
       </c>
-      <c r="F732" s="22"/>
+      <c r="F732" s="29"/>
     </row>
     <row r="733" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A733">
@@ -23628,7 +23640,7 @@
       <c r="D733" t="s">
         <v>1237</v>
       </c>
-      <c r="F733" s="22"/>
+      <c r="F733" s="29"/>
     </row>
     <row r="734" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A734">
@@ -23643,7 +23655,7 @@
       <c r="D734" t="s">
         <v>1238</v>
       </c>
-      <c r="F734" s="22"/>
+      <c r="F734" s="29"/>
     </row>
     <row r="735" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A735">
@@ -23658,7 +23670,7 @@
       <c r="D735" t="s">
         <v>1239</v>
       </c>
-      <c r="F735" s="22"/>
+      <c r="F735" s="29"/>
     </row>
     <row r="736" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A736">
@@ -23673,7 +23685,7 @@
       <c r="D736" t="s">
         <v>1240</v>
       </c>
-      <c r="F736" s="22"/>
+      <c r="F736" s="29"/>
     </row>
     <row r="737" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A737">
@@ -23688,7 +23700,7 @@
       <c r="D737" t="s">
         <v>1241</v>
       </c>
-      <c r="F737" s="22"/>
+      <c r="F737" s="29"/>
     </row>
     <row r="738" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A738">
@@ -23703,7 +23715,7 @@
       <c r="D738" t="s">
         <v>1242</v>
       </c>
-      <c r="F738" s="22"/>
+      <c r="F738" s="29"/>
     </row>
     <row r="739" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A739">
@@ -23718,7 +23730,7 @@
       <c r="D739" t="s">
         <v>1243</v>
       </c>
-      <c r="F739" s="22"/>
+      <c r="F739" s="29"/>
     </row>
     <row r="740" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A740">
@@ -23733,7 +23745,7 @@
       <c r="D740" t="s">
         <v>1244</v>
       </c>
-      <c r="F740" s="22"/>
+      <c r="F740" s="29"/>
     </row>
     <row r="741" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A741">
@@ -23748,7 +23760,7 @@
       <c r="D741" t="s">
         <v>1245</v>
       </c>
-      <c r="F741" s="22"/>
+      <c r="F741" s="29"/>
     </row>
     <row r="742" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A742">
@@ -23763,7 +23775,7 @@
       <c r="D742" t="s">
         <v>1246</v>
       </c>
-      <c r="F742" s="22"/>
+      <c r="F742" s="29"/>
     </row>
     <row r="743" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A743">
@@ -23778,7 +23790,7 @@
       <c r="D743" t="s">
         <v>1247</v>
       </c>
-      <c r="F743" s="22"/>
+      <c r="F743" s="29"/>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A744">
@@ -23793,7 +23805,7 @@
       <c r="D744" t="s">
         <v>1248</v>
       </c>
-      <c r="F744" s="22"/>
+      <c r="F744" s="29"/>
     </row>
     <row r="745" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A745">
@@ -26818,7 +26830,7 @@
       <c r="D960" t="s">
         <v>1455</v>
       </c>
-      <c r="E960" s="3"/>
+      <c r="E960" s="30"/>
     </row>
     <row r="961" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A961">
@@ -26833,7 +26845,7 @@
       <c r="D961" s="3" t="s">
         <v>1456</v>
       </c>
-      <c r="E961" s="3"/>
+      <c r="E961" s="30"/>
     </row>
     <row r="962" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A962">
@@ -26848,7 +26860,7 @@
       <c r="D962" s="3" t="s">
         <v>1457</v>
       </c>
-      <c r="E962" s="3"/>
+      <c r="E962" s="30"/>
     </row>
     <row r="963" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A963">
@@ -26863,7 +26875,7 @@
       <c r="D963" s="3" t="s">
         <v>1458</v>
       </c>
-      <c r="E963" s="3"/>
+      <c r="E963" s="30"/>
     </row>
     <row r="964" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A964">
@@ -26878,7 +26890,7 @@
       <c r="D964" s="3" t="s">
         <v>1459</v>
       </c>
-      <c r="E964" s="3"/>
+      <c r="E964" s="30"/>
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A965">
@@ -26893,7 +26905,7 @@
       <c r="D965" s="3" t="s">
         <v>1460</v>
       </c>
-      <c r="E965" s="3"/>
+      <c r="E965" s="30"/>
     </row>
     <row r="966" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A966">
@@ -26908,7 +26920,7 @@
       <c r="D966" s="3" t="s">
         <v>1461</v>
       </c>
-      <c r="E966" s="3"/>
+      <c r="E966" s="30"/>
     </row>
     <row r="967" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A967">
@@ -26923,7 +26935,7 @@
       <c r="D967" s="3" t="s">
         <v>1462</v>
       </c>
-      <c r="E967" s="3"/>
+      <c r="E967" s="30"/>
     </row>
     <row r="968" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A968">
@@ -26938,7 +26950,7 @@
       <c r="D968" s="3" t="s">
         <v>1463</v>
       </c>
-      <c r="E968" s="3"/>
+      <c r="E968" s="30"/>
     </row>
     <row r="969" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A969">
@@ -26953,7 +26965,7 @@
       <c r="D969" s="3" t="s">
         <v>1464</v>
       </c>
-      <c r="E969" s="3"/>
+      <c r="E969" s="30"/>
     </row>
     <row r="970" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A970">
@@ -26968,7 +26980,7 @@
       <c r="D970" s="3" t="s">
         <v>1465</v>
       </c>
-      <c r="E970" s="3"/>
+      <c r="E970" s="30"/>
     </row>
     <row r="971" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A971">
@@ -26983,7 +26995,7 @@
       <c r="D971" s="3" t="s">
         <v>1466</v>
       </c>
-      <c r="E971" s="3"/>
+      <c r="E971" s="30"/>
     </row>
     <row r="972" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A972">
@@ -26998,7 +27010,7 @@
       <c r="D972" s="3" t="s">
         <v>1467</v>
       </c>
-      <c r="E972" s="3"/>
+      <c r="E972" s="30"/>
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A973">
@@ -27013,7 +27025,7 @@
       <c r="D973" s="3" t="s">
         <v>1468</v>
       </c>
-      <c r="E973" s="3"/>
+      <c r="E973" s="30"/>
     </row>
     <row r="974" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A974">
@@ -27028,7 +27040,7 @@
       <c r="D974" s="3" t="s">
         <v>1469</v>
       </c>
-      <c r="E974" s="3"/>
+      <c r="E974" s="30"/>
     </row>
     <row r="975" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A975">
@@ -27043,7 +27055,7 @@
       <c r="D975" s="3" t="s">
         <v>1470</v>
       </c>
-      <c r="E975" s="3"/>
+      <c r="E975" s="30"/>
     </row>
     <row r="976" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A976">
@@ -27058,7 +27070,7 @@
       <c r="D976" s="3" t="s">
         <v>1471</v>
       </c>
-      <c r="E976" s="3"/>
+      <c r="E976" s="30"/>
     </row>
     <row r="977" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A977">
@@ -27073,7 +27085,7 @@
       <c r="D977" s="3" t="s">
         <v>1472</v>
       </c>
-      <c r="E977" s="3"/>
+      <c r="E977" s="30"/>
     </row>
     <row r="978" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A978">
@@ -27088,7 +27100,7 @@
       <c r="D978" s="3" t="s">
         <v>1473</v>
       </c>
-      <c r="E978" s="3"/>
+      <c r="E978" s="30"/>
     </row>
     <row r="979" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A979">
@@ -27103,7 +27115,7 @@
       <c r="D979" t="s">
         <v>1474</v>
       </c>
-      <c r="E979" s="3"/>
+      <c r="E979" s="30"/>
     </row>
     <row r="980" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A980">

</xml_diff>